<commit_message>
update design layout and add new table style
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -76,15 +76,15 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 60mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 60mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
@@ -100,33 +100,33 @@
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
     <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
+    <t>Kynol TR 100mg Capsule</t>
+  </si>
+  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -142,15 +142,15 @@
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
+    <t>Zithrox 15ml Suspension</t>
+  </si>
+  <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 15ml Suspension</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -169,21 +169,21 @@
     <t>100ml</t>
   </si>
   <si>
+    <t>36 's</t>
+  </si>
+  <si>
     <t>30 's</t>
   </si>
   <si>
-    <t>36 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
+    <t>4's</t>
+  </si>
+  <si>
     <t>5 's</t>
   </si>
   <si>
-    <t>4's</t>
-  </si>
-  <si>
     <t>60 's</t>
   </si>
   <si>
@@ -202,13 +202,13 @@
     <t>6 's</t>
   </si>
   <si>
+    <t>15 ml</t>
+  </si>
+  <si>
+    <t>30ml</t>
+  </si>
+  <si>
     <t>6's</t>
-  </si>
-  <si>
-    <t>30ml</t>
-  </si>
-  <si>
-    <t>15 ml</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -909,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
Add item stock days status table
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -76,54 +76,54 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 60mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 60mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 90mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+    <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
-    <t>Kynol D 25mg Tablet</t>
-  </si>
-  <si>
     <t>Kynol TR 100mg Capsule</t>
   </si>
   <si>
@@ -145,12 +145,12 @@
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -169,12 +169,12 @@
     <t>100ml</t>
   </si>
   <si>
+    <t>36 's</t>
+  </si>
+  <si>
     <t>30 's</t>
   </si>
   <si>
-    <t>36 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
@@ -205,10 +205,10 @@
     <t>6 's</t>
   </si>
   <si>
+    <t>30ml</t>
+  </si>
+  <si>
     <t>6's</t>
-  </si>
-  <si>
-    <t>30ml</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -858,7 +858,7 @@
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -909,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
update image and table position and size
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -76,57 +76,57 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 180mg Tablet</t>
+  </si>
+  <si>
+    <t>Dinafex 120mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 120mg Tablet</t>
-  </si>
-  <si>
-    <t>Dinafex 180mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule - 36's</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
-    <t>Ketonic 10mg Tablet</t>
-  </si>
-  <si>
     <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
+    <t>Kynol TR 100mg Capsule</t>
+  </si>
+  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -139,18 +139,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -160,30 +160,30 @@
     <t>50's</t>
   </si>
   <si>
+    <t>20's</t>
+  </si>
+  <si>
     <t>40's</t>
   </si>
   <si>
-    <t>20's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>30 's</t>
+  </si>
+  <si>
     <t>36 's</t>
   </si>
   <si>
-    <t>30 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
+    <t>4's</t>
+  </si>
+  <si>
     <t>5 's</t>
   </si>
   <si>
-    <t>4's</t>
-  </si>
-  <si>
     <t>60 's</t>
   </si>
   <si>
@@ -199,16 +199,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>30ml</t>
+  </si>
+  <si>
     <t>15 ml</t>
   </si>
   <si>
+    <t>6's</t>
+  </si>
+  <si>
     <t>6 's</t>
-  </si>
-  <si>
-    <t>30ml</t>
-  </si>
-  <si>
-    <t>6's</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -705,7 +705,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -909,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
update yesterday sales table
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -88,45 +88,45 @@
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule - 36's</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
-    <t>Ketonic 10mg Tablet</t>
-  </si>
-  <si>
     <t>Ketonic 30mg IM/IV Injection - 4's</t>
   </si>
   <si>
+    <t>Kynol D 25mg Tablet</t>
+  </si>
+  <si>
+    <t>Kynol TR 100mg Capsule</t>
+  </si>
+  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
-    <t>Kynol D 25mg Tablet</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -139,18 +139,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
-    <t>Zithrox 500mg Tablet</t>
+    <t>Zithrox 30ml Dry Suspension</t>
   </si>
   <si>
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -160,21 +160,21 @@
     <t>50's</t>
   </si>
   <si>
+    <t>20's</t>
+  </si>
+  <si>
     <t>40's</t>
   </si>
   <si>
-    <t>20's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>30 's</t>
+  </si>
+  <si>
     <t>36 's</t>
   </si>
   <si>
-    <t>30 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
@@ -184,12 +184,12 @@
     <t>4's</t>
   </si>
   <si>
+    <t>60 's</t>
+  </si>
+  <si>
     <t>50 's</t>
   </si>
   <si>
-    <t>60 's</t>
-  </si>
-  <si>
     <t>40 's</t>
   </si>
   <si>
@@ -199,16 +199,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>6 's</t>
+  </si>
+  <si>
     <t>15 ml</t>
   </si>
   <si>
-    <t>6 's</t>
+    <t>30ml</t>
   </si>
   <si>
     <t>6's</t>
-  </si>
-  <si>
-    <t>30ml</t>
   </si>
 </sst>
 </file>
@@ -807,7 +807,7 @@
         <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -858,7 +858,7 @@
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -909,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
Add Branch wise aging stock status table
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -76,48 +76,48 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 120mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 120mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 60mg Tablet - 40's</t>
+  </si>
+  <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 120mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 60mg Tablet - 40's</t>
-  </si>
-  <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
+    <t>Ketonic 30mg Injection</t>
+  </si>
+  <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg Injection</t>
-  </si>
-  <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
     <t>Kynol TR 100mg Capsule</t>
   </si>
   <si>
@@ -142,15 +142,15 @@
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
+    <t>Zithrox 15ml Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 30ml Dry Suspension</t>
   </si>
   <si>
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
-    <t>Zithrox 15ml Suspension</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -160,30 +160,30 @@
     <t>50's</t>
   </si>
   <si>
+    <t>40's</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
-    <t>40's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>36 's</t>
+  </si>
+  <si>
     <t>30 's</t>
   </si>
   <si>
-    <t>36 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
+    <t>4's</t>
+  </si>
+  <si>
     <t>5 's</t>
   </si>
   <si>
-    <t>4's</t>
-  </si>
-  <si>
     <t>50 's</t>
   </si>
   <si>
@@ -202,13 +202,13 @@
     <t>6's</t>
   </si>
   <si>
+    <t>15 ml</t>
+  </si>
+  <si>
     <t>30ml</t>
   </si>
   <si>
     <t>6 's</t>
-  </si>
-  <si>
-    <t>15 ml</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -807,7 +807,7 @@
         <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -909,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
Final update to go client
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -76,46 +76,49 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 180mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 180mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
     <t>Etorix 90mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule - 36's</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
     <t>Ketonic 30mg IM/IV Injection - 4's</t>
   </si>
   <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
-    <t>Ketonic 10mg Tablet</t>
+    <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
     <t>Kynol TR 100mg Capsule</t>
@@ -124,9 +127,6 @@
     <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
-    <t>Kynol TR 200mg Capsule</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -139,18 +139,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 15ml Suspension</t>
+  </si>
+  <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
-    <t>Zithrox 15ml Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 500mg Tablet</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -160,21 +160,21 @@
     <t>50's</t>
   </si>
   <si>
+    <t>20's</t>
+  </si>
+  <si>
     <t>40's</t>
   </si>
   <si>
-    <t>20's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>30 's</t>
+  </si>
+  <si>
     <t>36 's</t>
   </si>
   <si>
-    <t>30 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
@@ -199,16 +199,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>15 ml</t>
+  </si>
+  <si>
+    <t>30ml</t>
+  </si>
+  <si>
+    <t>6 's</t>
+  </si>
+  <si>
     <t>6's</t>
-  </si>
-  <si>
-    <t>15 ml</t>
-  </si>
-  <si>
-    <t>30ml</t>
-  </si>
-  <si>
-    <t>6 's</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -858,7 +858,7 @@
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -909,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
Arrange files in order and commenting code
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>BSL NO</t>
   </si>
@@ -67,6 +67,9 @@
     <t>Osticare</t>
   </si>
   <si>
+    <t>Rupaday</t>
+  </si>
+  <si>
     <t>Sk-Mox</t>
   </si>
   <si>
@@ -76,48 +79,48 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 120mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 120mg Tablet</t>
-  </si>
-  <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
+    <t>Etorix 60mg Tablet - 40's</t>
+  </si>
+  <si>
     <t>Etorix 120mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 60mg Tablet - 40's</t>
-  </si>
-  <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 30mg Injection</t>
+  </si>
+  <si>
     <t>Ketonic 30mg IM/IV Injection - 4's</t>
   </si>
   <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg Injection</t>
-  </si>
-  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
@@ -136,21 +139,24 @@
     <t>Osticare Tablet 24's</t>
   </si>
   <si>
+    <t>Rupaday Oral Solution 60ml</t>
+  </si>
+  <si>
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
     <t>Zithrox 30ml Dry Suspension</t>
   </si>
   <si>
-    <t>Zithrox 500mg Tablet</t>
-  </si>
-  <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -160,30 +166,30 @@
     <t>50's</t>
   </si>
   <si>
+    <t>40's</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
-    <t>40's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>36 's</t>
+  </si>
+  <si>
     <t>30 's</t>
   </si>
   <si>
-    <t>36 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
+    <t>5 's</t>
+  </si>
+  <si>
     <t>4's</t>
   </si>
   <si>
-    <t>5 's</t>
-  </si>
-  <si>
     <t>50 's</t>
   </si>
   <si>
@@ -196,19 +202,22 @@
     <t>24's</t>
   </si>
   <si>
+    <t>1's</t>
+  </si>
+  <si>
     <t>48 's</t>
   </si>
   <si>
+    <t>6's</t>
+  </si>
+  <si>
+    <t>6 's</t>
+  </si>
+  <si>
     <t>15 ml</t>
   </si>
   <si>
     <t>30ml</t>
-  </si>
-  <si>
-    <t>6 's</t>
-  </si>
-  <si>
-    <t>6's</t>
   </si>
 </sst>
 </file>
@@ -566,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,10 +609,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -617,10 +626,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -634,10 +643,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -651,10 +660,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -668,10 +677,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -685,7 +694,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>48</v>
@@ -702,10 +711,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -719,10 +728,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -736,10 +745,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -753,10 +762,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -770,10 +779,10 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -787,10 +796,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -804,10 +813,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -821,10 +830,10 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -838,10 +847,10 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -855,10 +864,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -872,10 +881,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -889,10 +898,10 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -906,10 +915,10 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -923,10 +932,10 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -940,15 +949,15 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -957,15 +966,15 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -974,10 +983,10 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -985,16 +994,16 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1002,16 +1011,16 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1019,16 +1028,33 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dashboard.png, banner_ai.png and cumilative sales target
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -79,57 +79,57 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 180mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 180mg Tablet</t>
-  </si>
-  <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 60mg Tablet - 40's</t>
+  </si>
+  <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 120mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 60mg Tablet - 40's</t>
-  </si>
-  <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
     <t>Ketonic 30mg IM/IV Injection - 4's</t>
   </si>
   <si>
+    <t>Ketonic 30mg Injection</t>
+  </si>
+  <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg Injection</t>
-  </si>
-  <si>
     <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
+    <t>Kynol TR 100mg Capsule</t>
+  </si>
+  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -148,15 +148,15 @@
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
     <t>Zithrox 30ml Dry Suspension</t>
   </si>
   <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -166,21 +166,21 @@
     <t>50's</t>
   </si>
   <si>
+    <t>40's</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
-    <t>40's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>36 's</t>
+  </si>
+  <si>
     <t>30 's</t>
   </si>
   <si>
-    <t>36 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
@@ -211,13 +211,13 @@
     <t>15 ml</t>
   </si>
   <si>
+    <t>6's</t>
+  </si>
+  <si>
     <t>6 's</t>
   </si>
   <si>
     <t>30ml</t>
-  </si>
-  <si>
-    <t>6's</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -731,7 +731,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -833,7 +833,7 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -850,7 +850,7 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -884,7 +884,7 @@
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -901,7 +901,7 @@
         <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -918,7 +918,7 @@
         <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
update Branch - Brand - SKU wise Stock Aging Status: Summary
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -79,27 +79,27 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 120mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 120mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 60mg Tablet - 40's</t>
+  </si>
+  <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 120mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 60mg Tablet - 40's</t>
-  </si>
-  <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
@@ -115,21 +115,21 @@
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
+    <t>Kynol TR 100mg Capsule</t>
+  </si>
+  <si>
     <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -145,18 +145,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
-    <t>Zithrox 500mg Tablet</t>
-  </si>
-  <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -166,12 +166,12 @@
     <t>50's</t>
   </si>
   <si>
+    <t>40's</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
-    <t>40's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
@@ -190,12 +190,12 @@
     <t>4's</t>
   </si>
   <si>
+    <t>50 's</t>
+  </si>
+  <si>
     <t>60 's</t>
   </si>
   <si>
-    <t>50 's</t>
-  </si>
-  <si>
     <t>40 's</t>
   </si>
   <si>
@@ -208,16 +208,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>6 's</t>
+  </si>
+  <si>
+    <t>30ml</t>
+  </si>
+  <si>
     <t>6's</t>
   </si>
   <si>
     <t>15 ml</t>
-  </si>
-  <si>
-    <t>6 's</t>
-  </si>
-  <si>
-    <t>30ml</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -731,7 +731,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -833,7 +833,7 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -850,7 +850,7 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>

<commit_message>
Mater update 22 nov 2020
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -79,48 +79,48 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 60mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 60mg Tablet</t>
-  </si>
-  <si>
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
     <t>Etorix 90mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule - 36's</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
-    <t>Ketonic 10mg Tablet</t>
-  </si>
-  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
@@ -145,18 +145,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
-    <t>Zithrox 30ml Dry Suspension</t>
+    <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
-    <t>Zithrox 15ml Suspension</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -166,30 +166,30 @@
     <t>50's</t>
   </si>
   <si>
+    <t>20's</t>
+  </si>
+  <si>
     <t>40's</t>
   </si>
   <si>
-    <t>20's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
+    <t>30 's</t>
+  </si>
+  <si>
     <t>36 's</t>
   </si>
   <si>
-    <t>30 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
+    <t>4's</t>
+  </si>
+  <si>
     <t>5 's</t>
   </si>
   <si>
-    <t>4's</t>
-  </si>
-  <si>
     <t>50 's</t>
   </si>
   <si>
@@ -208,16 +208,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>30ml</t>
+  </si>
+  <si>
     <t>6 's</t>
   </si>
   <si>
-    <t>30ml</t>
+    <t>15 ml</t>
   </si>
   <si>
     <t>6's</t>
-  </si>
-  <si>
-    <t>15 ml</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -731,7 +731,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -833,7 +833,7 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -850,7 +850,7 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -867,7 +867,7 @@
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -918,7 +918,7 @@
         <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
update DB connections and arrange all code
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -79,46 +79,49 @@
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 120mg Tablet</t>
+  </si>
+  <si>
+    <t>Dinafex 180mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 120mg Tablet</t>
-  </si>
-  <si>
-    <t>Dinafex 180mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 120mg Tablet</t>
   </si>
   <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
+    <t>Ketonic 30mg Injection</t>
+  </si>
+  <si>
     <t>Ketonic 30mg IM/IV Injection - 4's</t>
   </si>
   <si>
-    <t>Ketonic 10mg Tablet</t>
-  </si>
-  <si>
-    <t>Ketonic 30mg Injection</t>
+    <t>Kynol D 25mg Tablet</t>
   </si>
   <si>
     <t>Kynol TR 200mg Capsule</t>
@@ -127,9 +130,6 @@
     <t>Kynol TR 100mg Capsule</t>
   </si>
   <si>
-    <t>Kynol D 25mg Tablet</t>
-  </si>
-  <si>
     <t>Naprox Plus 500mg Tablet - 30's</t>
   </si>
   <si>
@@ -145,18 +145,18 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 15ml Suspension</t>
+  </si>
+  <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
     <t>Zithrox 30ml Dry Suspension</t>
   </si>
   <si>
-    <t>Zithrox 500mg Tablet</t>
-  </si>
-  <si>
-    <t>Zithrox 15ml Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
-  </si>
-  <si>
     <t>60 ml</t>
   </si>
   <si>
@@ -175,27 +175,27 @@
     <t>100ml</t>
   </si>
   <si>
+    <t>36 's</t>
+  </si>
+  <si>
     <t>30 's</t>
   </si>
   <si>
-    <t>36 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
+    <t>5 's</t>
+  </si>
+  <si>
     <t>4's</t>
   </si>
   <si>
-    <t>5 's</t>
+    <t>60 's</t>
   </si>
   <si>
     <t>50 's</t>
   </si>
   <si>
-    <t>60 's</t>
-  </si>
-  <si>
     <t>40 's</t>
   </si>
   <si>
@@ -208,16 +208,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>15 ml</t>
+  </si>
+  <si>
+    <t>6's</t>
+  </si>
+  <si>
+    <t>6 's</t>
+  </si>
+  <si>
     <t>30ml</t>
-  </si>
-  <si>
-    <t>6 's</t>
-  </si>
-  <si>
-    <t>15 ml</t>
-  </si>
-  <si>
-    <t>6's</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -714,7 +714,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -731,7 +731,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -816,7 +816,7 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -833,7 +833,7 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -867,7 +867,7 @@
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -884,7 +884,7 @@
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -918,7 +918,7 @@
         <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
Update all for v 15
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>BSL NO</t>
   </si>
@@ -31,6 +31,9 @@
     <t>UOM</t>
   </si>
   <si>
+    <t>Biltin</t>
+  </si>
+  <si>
     <t>Desodin</t>
   </si>
   <si>
@@ -76,30 +79,33 @@
     <t>Zithrox</t>
   </si>
   <si>
+    <t>Biltin 20mg Tablet 30's</t>
+  </si>
+  <si>
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 180mg Tablet</t>
+  </si>
+  <si>
+    <t>Dinafex 120mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 60mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 180mg Tablet</t>
-  </si>
-  <si>
-    <t>Dinafex 120mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 90mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 120mg Tablet</t>
   </si>
   <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
@@ -112,15 +118,15 @@
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 30mg Injection</t>
+  </si>
+  <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
     <t>Ketonic 30mg IM/IV Injection - 4's</t>
   </si>
   <si>
-    <t>Ketonic 10mg Tablet</t>
-  </si>
-  <si>
-    <t>Ketonic 30mg Injection</t>
-  </si>
-  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
@@ -157,12 +163,12 @@
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
+    <t>30's</t>
+  </si>
+  <si>
     <t>60 ml</t>
   </si>
   <si>
-    <t>30's</t>
-  </si>
-  <si>
     <t>50's</t>
   </si>
   <si>
@@ -184,10 +190,10 @@
     <t>8 's</t>
   </si>
   <si>
+    <t>5 's</t>
+  </si>
+  <si>
     <t>4's</t>
-  </si>
-  <si>
-    <t>5 's</t>
   </si>
   <si>
     <t>60 's</t>
@@ -575,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,7 +606,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -609,15 +615,15 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -626,10 +632,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -637,16 +643,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -654,21 +660,21 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -677,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>49</v>
@@ -685,7 +691,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -694,10 +700,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -705,16 +711,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -722,21 +728,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -745,15 +751,15 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -762,10 +768,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -773,21 +779,21 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -796,15 +802,15 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -813,10 +819,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -824,16 +830,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -841,21 +847,21 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -864,10 +870,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -875,16 +881,16 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -892,21 +898,21 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -915,15 +921,15 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -932,15 +938,15 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
@@ -949,15 +955,15 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -966,15 +972,15 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -983,15 +989,15 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -1000,10 +1006,10 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1011,16 +1017,16 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1028,16 +1034,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1045,16 +1051,33 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add static target and sales data in stacked bar chart
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>BSL NO</t>
   </si>
@@ -31,9 +31,6 @@
     <t>UOM</t>
   </si>
   <si>
-    <t>Biltin</t>
-  </si>
-  <si>
     <t>Desodin</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Zithrox</t>
   </si>
   <si>
-    <t>Biltin 20mg Tablet 30's</t>
-  </si>
-  <si>
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
@@ -97,15 +91,15 @@
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 60mg Tablet - 40's</t>
+  </si>
+  <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 90mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
-    <t>Etorix 60mg Tablet - 40's</t>
-  </si>
-  <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
@@ -121,12 +115,12 @@
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
+    <t>Ketonic 30mg IM/IV Injection - 4's</t>
+  </si>
+  <si>
     <t>Ketonic 10mg Tablet</t>
   </si>
   <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
@@ -151,33 +145,33 @@
     <t>Sk-Mox 500mg Capsule</t>
   </si>
   <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
+    <t>Zithrox 250mg Tablet - 6's</t>
+  </si>
+  <si>
+    <t>Zithrox 500mg Tablet</t>
+  </si>
+  <si>
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
-    <t>Zithrox 500mg Tablet</t>
-  </si>
-  <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
+    <t>60 ml</t>
   </si>
   <si>
     <t>30's</t>
   </si>
   <si>
-    <t>60 ml</t>
-  </si>
-  <si>
     <t>50's</t>
   </si>
   <si>
+    <t>40's</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
-    <t>40's</t>
-  </si>
-  <si>
     <t>100ml</t>
   </si>
   <si>
@@ -214,16 +208,16 @@
     <t>48 's</t>
   </si>
   <si>
+    <t>30ml</t>
+  </si>
+  <si>
+    <t>6's</t>
+  </si>
+  <si>
+    <t>6 's</t>
+  </si>
+  <si>
     <t>15 ml</t>
-  </si>
-  <si>
-    <t>6 's</t>
-  </si>
-  <si>
-    <t>30ml</t>
-  </si>
-  <si>
-    <t>6's</t>
   </si>
 </sst>
 </file>
@@ -581,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -606,7 +600,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -615,15 +609,15 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -632,10 +626,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -643,16 +637,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -660,21 +654,21 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -683,7 +677,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>49</v>
@@ -691,7 +685,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -700,10 +694,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -711,16 +705,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -728,21 +722,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -751,15 +745,15 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -768,10 +762,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -779,21 +773,21 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -802,15 +796,15 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -819,10 +813,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -830,16 +824,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -847,21 +841,21 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -870,10 +864,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -881,16 +875,16 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -898,21 +892,21 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -921,15 +915,15 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -938,15 +932,15 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
@@ -955,15 +949,15 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -972,15 +966,15 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -989,15 +983,15 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -1006,10 +1000,10 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1017,16 +1011,16 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1034,16 +1028,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1051,33 +1045,16 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29">
-        <v>28</v>
-      </c>
-      <c r="D29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add scheduler in coding sections
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>BSL NO</t>
   </si>
@@ -31,9 +31,6 @@
     <t>UOM</t>
   </si>
   <si>
-    <t>Biltin</t>
-  </si>
-  <si>
     <t>Desodin</t>
   </si>
   <si>
@@ -79,60 +76,57 @@
     <t>Zithrox</t>
   </si>
   <si>
-    <t>Biltin 20mg Tablet 30's</t>
-  </si>
-  <si>
     <t>Desodin 60ml Syrup</t>
   </si>
   <si>
+    <t>Dinafex 60mg Tablet</t>
+  </si>
+  <si>
     <t>Dinafex 180mg Tablet</t>
   </si>
   <si>
     <t>Dinafex 120mg Tablet</t>
   </si>
   <si>
-    <t>Dinafex 60mg Tablet</t>
-  </si>
-  <si>
     <t>Dorenta 50mg Tablet</t>
   </si>
   <si>
+    <t>Etorix 120mg Tablet</t>
+  </si>
+  <si>
     <t>Etorix 90mg Tablet</t>
   </si>
   <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
     <t>Etorix 60mg Tablet - 40's</t>
   </si>
   <si>
     <t>Fenobac 100ml Syrup</t>
   </si>
   <si>
+    <t>Flucloxin 500mg Capsule - 36's</t>
+  </si>
+  <si>
     <t>Flucloxin 500mg Capsule</t>
   </si>
   <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
     <t>Geminox 320mg Tablet - 8's</t>
   </si>
   <si>
+    <t>Ketonic 10mg Tablet</t>
+  </si>
+  <si>
     <t>Ketonic 30mg Injection</t>
   </si>
   <si>
-    <t>Ketonic 10mg Tablet</t>
-  </si>
-  <si>
     <t>Ketonic 30mg IM/IV Injection - 4's</t>
   </si>
   <si>
+    <t>Kynol D 25mg Tablet</t>
+  </si>
+  <si>
     <t>Kynol TR 200mg Capsule</t>
   </si>
   <si>
-    <t>Kynol D 25mg Tablet</t>
-  </si>
-  <si>
     <t>Kynol TR 100mg Capsule</t>
   </si>
   <si>
@@ -154,21 +148,21 @@
     <t>Zithrox 15ml Suspension</t>
   </si>
   <si>
+    <t>Zithrox 30ml Dry Suspension</t>
+  </si>
+  <si>
     <t>Zithrox 500mg Tablet</t>
   </si>
   <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
     <t>Zithrox 250mg Tablet - 6's</t>
   </si>
   <si>
+    <t>60 ml</t>
+  </si>
+  <si>
     <t>30's</t>
   </si>
   <si>
-    <t>60 ml</t>
-  </si>
-  <si>
     <t>50's</t>
   </si>
   <si>
@@ -181,12 +175,12 @@
     <t>100ml</t>
   </si>
   <si>
+    <t>36 's</t>
+  </si>
+  <si>
     <t>30 's</t>
   </si>
   <si>
-    <t>36 's</t>
-  </si>
-  <si>
     <t>8 's</t>
   </si>
   <si>
@@ -217,10 +211,10 @@
     <t>15 ml</t>
   </si>
   <si>
+    <t>30ml</t>
+  </si>
+  <si>
     <t>6 's</t>
-  </si>
-  <si>
-    <t>30ml</t>
   </si>
   <si>
     <t>6's</t>
@@ -581,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -606,7 +600,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -615,15 +609,15 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -632,10 +626,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -643,16 +637,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -660,21 +654,21 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -683,7 +677,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>49</v>
@@ -691,7 +685,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -700,10 +694,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -711,16 +705,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -728,21 +722,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -751,15 +745,15 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -768,10 +762,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -779,21 +773,21 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -802,15 +796,15 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -819,10 +813,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -830,16 +824,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -847,21 +841,21 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -870,10 +864,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -881,16 +875,16 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -898,21 +892,21 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -921,15 +915,15 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -938,15 +932,15 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
@@ -955,15 +949,15 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -972,15 +966,15 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -989,15 +983,15 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -1006,10 +1000,10 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1017,16 +1011,16 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1034,16 +1028,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1051,33 +1045,16 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29">
-        <v>28</v>
-      </c>
-      <c r="D29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all target vs sales chart
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>BSL NO</t>
   </si>
@@ -31,157 +31,121 @@
     <t>UOM</t>
   </si>
   <si>
-    <t>Aldorin</t>
-  </si>
-  <si>
-    <t>Cardobis</t>
-  </si>
-  <si>
-    <t>Cardon</t>
-  </si>
-  <si>
-    <t>Cardoneb</t>
-  </si>
-  <si>
-    <t>Cardovan</t>
-  </si>
-  <si>
-    <t>Dialon</t>
-  </si>
-  <si>
-    <t>Edenil</t>
-  </si>
-  <si>
-    <t>GLIKAZID</t>
-  </si>
-  <si>
-    <t>Ligazid</t>
-  </si>
-  <si>
-    <t>Lipicon</t>
-  </si>
-  <si>
-    <t>Noclog</t>
-  </si>
-  <si>
-    <t>Pivasta</t>
-  </si>
-  <si>
-    <t>Sidopin</t>
-  </si>
-  <si>
-    <t>Sitazid</t>
-  </si>
-  <si>
-    <t>Aldorin 50mg Tablet - 24's</t>
-  </si>
-  <si>
-    <t>Cardobis 2.5 FC Tablet 30's</t>
-  </si>
-  <si>
-    <t>Cardoplus 50mg Tablet 30's</t>
-  </si>
-  <si>
-    <t>Cardoplus 50mg Tablet</t>
-  </si>
-  <si>
-    <t>Cardoneb 5 FC Tablet 30's</t>
-  </si>
-  <si>
-    <t>Cardoneb 2.5 FC Tablet 30's</t>
-  </si>
-  <si>
-    <t>Cardovan 160mg Tablet 30's</t>
-  </si>
-  <si>
-    <t>Cardovan 80mg Tablet 30's</t>
-  </si>
-  <si>
-    <t>Cardovan Plus 80/12.5 Tablet 30's</t>
-  </si>
-  <si>
-    <t>Cardovan Plus 160/12.5 Tablet 30's</t>
-  </si>
-  <si>
-    <t>Dialon 4mg Tablet</t>
-  </si>
-  <si>
-    <t>Edenil 20mg Tablet</t>
-  </si>
-  <si>
-    <t>Glikazid 80mg Tablet 30's</t>
-  </si>
-  <si>
-    <t>Ligazid 5mg Tablet 10's</t>
-  </si>
-  <si>
-    <t>Ligazid 5mg Tablet 20's</t>
-  </si>
-  <si>
-    <t>Ligazid M 2.5/500</t>
-  </si>
-  <si>
-    <t>Lipicon 40mg Tablet - 10's</t>
-  </si>
-  <si>
-    <t>Lipicon 10mg Tablet Container 30's</t>
-  </si>
-  <si>
-    <t>Lipicon 20mg Tablet - 20's</t>
-  </si>
-  <si>
-    <t>Lipicon 10mg Tablet - 40's</t>
-  </si>
-  <si>
-    <t>Noclog 75mg Tablet</t>
-  </si>
-  <si>
-    <t>Noclog Plus 75mg Tablet</t>
-  </si>
-  <si>
-    <t>Noclog 75mg Tablet 30's</t>
-  </si>
-  <si>
-    <t>Noclog Plus Tablet 30's</t>
-  </si>
-  <si>
-    <t>Pivasta 2mg Tablet 20's</t>
-  </si>
-  <si>
-    <t>Sidoplus 50mg Tablet</t>
-  </si>
-  <si>
-    <t>Sitazid 50mg Tablet 20's</t>
-  </si>
-  <si>
-    <t>Sitazid 100mg Tablet 10's</t>
-  </si>
-  <si>
-    <t>24's</t>
+    <t>Esoral</t>
+  </si>
+  <si>
+    <t>Losectil</t>
+  </si>
+  <si>
+    <t>Rabifast</t>
+  </si>
+  <si>
+    <t>Softi</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Tablet</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Capsule 50's</t>
+  </si>
+  <si>
+    <t>Esoral 40mg EC Tablet - 42's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Tablet  80's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Tablet - 50's</t>
+  </si>
+  <si>
+    <t>Esoral Injection &amp; MUPS 20</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Capsule Container 30's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg  Tablet 100's</t>
+  </si>
+  <si>
+    <t>Esoral Injection &amp; Capsule 20</t>
+  </si>
+  <si>
+    <t>Esoral 40mg Tablet</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Capsule (100's)</t>
+  </si>
+  <si>
+    <t>Losectil 10mg Capsule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Losectil DR Tablet </t>
+  </si>
+  <si>
+    <t>Losectil 20mg Powder for Oral Suspension</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Powder for Oral Suspension - 30's</t>
+  </si>
+  <si>
+    <t>Losectil 40mg Powder for Oral Suspension</t>
+  </si>
+  <si>
+    <t>Losectil 40mg Capsule (24's)</t>
+  </si>
+  <si>
+    <t>Losectil 40mg Capsule - 48's</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Capsule 500s</t>
+  </si>
+  <si>
+    <t>Rabifast 20mg Tablet - 50's</t>
+  </si>
+  <si>
+    <t>Softi Ointment 15gm</t>
+  </si>
+  <si>
+    <t>20's</t>
+  </si>
+  <si>
+    <t>50's</t>
+  </si>
+  <si>
+    <t>42's</t>
+  </si>
+  <si>
+    <t>80's</t>
+  </si>
+  <si>
+    <t>Bundle</t>
   </si>
   <si>
     <t>30's</t>
   </si>
   <si>
-    <t>20 's</t>
-  </si>
-  <si>
-    <t>20'S</t>
-  </si>
-  <si>
-    <t>30 's</t>
-  </si>
-  <si>
-    <t>10's</t>
-  </si>
-  <si>
-    <t>20's</t>
-  </si>
-  <si>
-    <t>10 's</t>
-  </si>
-  <si>
-    <t>40 's</t>
+    <t>100's</t>
+  </si>
+  <si>
+    <t>100 's</t>
+  </si>
+  <si>
+    <t>48 's</t>
+  </si>
+  <si>
+    <t>60 's</t>
+  </si>
+  <si>
+    <t>24 's</t>
+  </si>
+  <si>
+    <t>48's</t>
+  </si>
+  <si>
+    <t>500's</t>
+  </si>
+  <si>
+    <t>15gm</t>
   </si>
 </sst>
 </file>
@@ -539,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,7 +528,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -573,469 +537,350 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24">
-        <v>23</v>
-      </c>
-      <c r="D24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>20</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
         <v>43</v>
-      </c>
-      <c r="E26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29">
-        <v>28</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add last months data in details table
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -43,106 +43,106 @@
     <t>Softi</t>
   </si>
   <si>
+    <t>Esoral Injection &amp; Capsule 20</t>
+  </si>
+  <si>
     <t>Esoral 20mg Tablet</t>
   </si>
   <si>
+    <t>Esoral 40mg Tablet</t>
+  </si>
+  <si>
+    <t>Esoral Injection &amp; MUPS 20</t>
+  </si>
+  <si>
     <t>Esoral 20mg Capsule 50's</t>
   </si>
   <si>
+    <t>Esoral 20mg Tablet - 50's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Tablet  80's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg  Tablet 100's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Capsule Container 30's</t>
+  </si>
+  <si>
     <t>Esoral 40mg EC Tablet - 42's</t>
   </si>
   <si>
-    <t>Esoral 20mg Tablet  80's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Tablet - 50's</t>
-  </si>
-  <si>
-    <t>Esoral Injection &amp; MUPS 20</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Capsule Container 30's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg  Tablet 100's</t>
-  </si>
-  <si>
-    <t>Esoral Injection &amp; Capsule 20</t>
-  </si>
-  <si>
-    <t>Esoral 40mg Tablet</t>
+    <t>Losectil 20mg Capsule 500s</t>
+  </si>
+  <si>
+    <t>Losectil 10mg Capsule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Losectil DR Tablet </t>
+  </si>
+  <si>
+    <t>Losectil 40mg Capsule (24's)</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Powder for Oral Suspension</t>
+  </si>
+  <si>
+    <t>Losectil 40mg Powder for Oral Suspension</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Powder for Oral Suspension - 30's</t>
+  </si>
+  <si>
+    <t>Losectil 40mg Capsule - 48's</t>
   </si>
   <si>
     <t>Losectil 20mg Capsule (100's)</t>
   </si>
   <si>
-    <t>Losectil 10mg Capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Losectil DR Tablet </t>
-  </si>
-  <si>
-    <t>Losectil 20mg Powder for Oral Suspension</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Powder for Oral Suspension - 30's</t>
-  </si>
-  <si>
-    <t>Losectil 40mg Powder for Oral Suspension</t>
-  </si>
-  <si>
-    <t>Losectil 40mg Capsule (24's)</t>
-  </si>
-  <si>
-    <t>Losectil 40mg Capsule - 48's</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Capsule 500s</t>
-  </si>
-  <si>
     <t>Rabifast 20mg Tablet - 50's</t>
   </si>
   <si>
     <t>Softi Ointment 15gm</t>
   </si>
   <si>
+    <t>Bundle</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
     <t>50's</t>
   </si>
   <si>
+    <t>80's</t>
+  </si>
+  <si>
+    <t>100's</t>
+  </si>
+  <si>
+    <t>30's</t>
+  </si>
+  <si>
     <t>42's</t>
   </si>
   <si>
-    <t>80's</t>
-  </si>
-  <si>
-    <t>Bundle</t>
-  </si>
-  <si>
-    <t>30's</t>
-  </si>
-  <si>
-    <t>100's</t>
+    <t>500's</t>
+  </si>
+  <si>
+    <t>48 's</t>
+  </si>
+  <si>
+    <t>60 's</t>
+  </si>
+  <si>
+    <t>24 's</t>
+  </si>
+  <si>
+    <t>48's</t>
   </si>
   <si>
     <t>100 's</t>
-  </si>
-  <si>
-    <t>48 's</t>
-  </si>
-  <si>
-    <t>60 's</t>
-  </si>
-  <si>
-    <t>24 's</t>
-  </si>
-  <si>
-    <t>48's</t>
-  </si>
-  <si>
-    <t>500's</t>
   </si>
   <si>
     <t>15gm</t>
@@ -574,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -591,7 +591,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -608,7 +608,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -625,7 +625,7 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -642,7 +642,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -676,7 +676,7 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -693,7 +693,7 @@
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -761,7 +761,7 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -778,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -795,7 +795,7 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -812,7 +812,7 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -863,7 +863,7 @@
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:5">

</xml_diff>

<commit_message>
update last data update time in banner_code.py
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -43,106 +43,106 @@
     <t>Softi</t>
   </si>
   <si>
+    <t>Esoral 20mg Capsule 50's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Tablet  80's</t>
+  </si>
+  <si>
     <t>Esoral Injection &amp; Capsule 20</t>
   </si>
   <si>
+    <t>Esoral 20mg Capsule Container 30's</t>
+  </si>
+  <si>
+    <t>Esoral 20mg Tablet - 50's</t>
+  </si>
+  <si>
+    <t>Esoral 40mg Tablet</t>
+  </si>
+  <si>
+    <t>Esoral 40mg EC Tablet - 42's</t>
+  </si>
+  <si>
     <t>Esoral 20mg Tablet</t>
   </si>
   <si>
-    <t>Esoral 40mg Tablet</t>
+    <t>Esoral 20mg  Tablet 100's</t>
   </si>
   <si>
     <t>Esoral Injection &amp; MUPS 20</t>
   </si>
   <si>
-    <t>Esoral 20mg Capsule 50's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Tablet - 50's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Tablet  80's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg  Tablet 100's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Capsule Container 30's</t>
-  </si>
-  <si>
-    <t>Esoral 40mg EC Tablet - 42's</t>
+    <t>Losectil 40mg Capsule (24's)</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Powder for Oral Suspension - 30's</t>
+  </si>
+  <si>
+    <t>Losectil 10mg Capsule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Losectil DR Tablet </t>
+  </si>
+  <si>
+    <t>Losectil 40mg Powder for Oral Suspension</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Powder for Oral Suspension</t>
+  </si>
+  <si>
+    <t>Losectil 40mg Capsule - 48's</t>
+  </si>
+  <si>
+    <t>Losectil 20mg Capsule (100's)</t>
   </si>
   <si>
     <t>Losectil 20mg Capsule 500s</t>
   </si>
   <si>
-    <t>Losectil 10mg Capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Losectil DR Tablet </t>
-  </si>
-  <si>
-    <t>Losectil 40mg Capsule (24's)</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Powder for Oral Suspension</t>
-  </si>
-  <si>
-    <t>Losectil 40mg Powder for Oral Suspension</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Powder for Oral Suspension - 30's</t>
-  </si>
-  <si>
-    <t>Losectil 40mg Capsule - 48's</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Capsule (100's)</t>
-  </si>
-  <si>
     <t>Rabifast 20mg Tablet - 50's</t>
   </si>
   <si>
     <t>Softi Ointment 15gm</t>
   </si>
   <si>
+    <t>50's</t>
+  </si>
+  <si>
+    <t>80's</t>
+  </si>
+  <si>
     <t>Bundle</t>
   </si>
   <si>
+    <t>30's</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
-    <t>50's</t>
-  </si>
-  <si>
-    <t>80's</t>
+    <t>42's</t>
   </si>
   <si>
     <t>100's</t>
   </si>
   <si>
-    <t>30's</t>
-  </si>
-  <si>
-    <t>42's</t>
+    <t>24 's</t>
+  </si>
+  <si>
+    <t>48 's</t>
+  </si>
+  <si>
+    <t>60 's</t>
+  </si>
+  <si>
+    <t>48's</t>
+  </si>
+  <si>
+    <t>100 's</t>
   </si>
   <si>
     <t>500's</t>
-  </si>
-  <si>
-    <t>48 's</t>
-  </si>
-  <si>
-    <t>60 's</t>
-  </si>
-  <si>
-    <t>24 's</t>
-  </si>
-  <si>
-    <t>48's</t>
-  </si>
-  <si>
-    <t>100 's</t>
   </si>
   <si>
     <t>15gm</t>
@@ -528,7 +528,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -574,12 +574,12 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -591,12 +591,12 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -608,12 +608,12 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -625,12 +625,12 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -642,12 +642,12 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -676,12 +676,12 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -693,12 +693,12 @@
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -727,12 +727,12 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -744,12 +744,12 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -761,12 +761,12 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -778,12 +778,12 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -795,12 +795,12 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -812,12 +812,12 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -863,12 +863,12 @@
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fix target related bugs
</commit_message>
<xml_diff>
--- a/Data/NoSales.xlsx
+++ b/Data/NoSales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>BSL NO</t>
   </si>
@@ -31,121 +31,121 @@
     <t>UOM</t>
   </si>
   <si>
-    <t>Esoral</t>
-  </si>
-  <si>
-    <t>Losectil</t>
-  </si>
-  <si>
-    <t>Rabifast</t>
-  </si>
-  <si>
-    <t>Softi</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Capsule 50's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Tablet  80's</t>
-  </si>
-  <si>
-    <t>Esoral Injection &amp; Capsule 20</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Capsule Container 30's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Tablet - 50's</t>
-  </si>
-  <si>
-    <t>Esoral 40mg Tablet</t>
-  </si>
-  <si>
-    <t>Esoral 40mg EC Tablet - 42's</t>
-  </si>
-  <si>
-    <t>Esoral 20mg Tablet</t>
-  </si>
-  <si>
-    <t>Esoral 20mg  Tablet 100's</t>
-  </si>
-  <si>
-    <t>Esoral Injection &amp; MUPS 20</t>
-  </si>
-  <si>
-    <t>Losectil 40mg Capsule (24's)</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Powder for Oral Suspension - 30's</t>
-  </si>
-  <si>
-    <t>Losectil 10mg Capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Losectil DR Tablet </t>
-  </si>
-  <si>
-    <t>Losectil 40mg Powder for Oral Suspension</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Powder for Oral Suspension</t>
-  </si>
-  <si>
-    <t>Losectil 40mg Capsule - 48's</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Capsule (100's)</t>
-  </si>
-  <si>
-    <t>Losectil 20mg Capsule 500s</t>
-  </si>
-  <si>
-    <t>Rabifast 20mg Tablet - 50's</t>
-  </si>
-  <si>
-    <t>Softi Ointment 15gm</t>
-  </si>
-  <si>
-    <t>50's</t>
-  </si>
-  <si>
-    <t>80's</t>
-  </si>
-  <si>
-    <t>Bundle</t>
+    <t>Aldorin</t>
+  </si>
+  <si>
+    <t>Cardoneb</t>
+  </si>
+  <si>
+    <t>Cardovan</t>
+  </si>
+  <si>
+    <t>Dialon</t>
+  </si>
+  <si>
+    <t>GLIKAZID</t>
+  </si>
+  <si>
+    <t>Irbes</t>
+  </si>
+  <si>
+    <t>Ligazid</t>
+  </si>
+  <si>
+    <t>Lipicon</t>
+  </si>
+  <si>
+    <t>Pivasta</t>
+  </si>
+  <si>
+    <t>Sitazid</t>
+  </si>
+  <si>
+    <t>Aldorin 50mg Tablet - 24's</t>
+  </si>
+  <si>
+    <t>Cardoneb 5 FC Tablet 30's</t>
+  </si>
+  <si>
+    <t>Cardoneb 2.5 FC Tablet 30's</t>
+  </si>
+  <si>
+    <t>Cardovan Plus 80/12.5 Tablet 30's</t>
+  </si>
+  <si>
+    <t>Cardovan 160mg Tablet 30's</t>
+  </si>
+  <si>
+    <t>Cardovan 80mg Tablet 30's</t>
+  </si>
+  <si>
+    <t>Cardovan Plus 160/12.5 Tablet 30's</t>
+  </si>
+  <si>
+    <t>Dialon 4mg Tablet</t>
+  </si>
+  <si>
+    <t>Glikazid 80mg Tablet 30's</t>
+  </si>
+  <si>
+    <t>Irbes 75mg Tablet</t>
+  </si>
+  <si>
+    <t>Ligazid 5mg Tablet 20's</t>
+  </si>
+  <si>
+    <t>Ligazid 5mg Tablet 10's</t>
+  </si>
+  <si>
+    <t>Ligazid M 2.5/500</t>
+  </si>
+  <si>
+    <t>Lipicon 20mg Tablet - 20's</t>
+  </si>
+  <si>
+    <t>Lipicon 10mg Tablet Container 30's</t>
+  </si>
+  <si>
+    <t>Lipicon 40mg Tablet - 10's</t>
+  </si>
+  <si>
+    <t>Lipicon 10mg Tablet - 40's</t>
+  </si>
+  <si>
+    <t>Pivasta 2mg Tablet 20's</t>
+  </si>
+  <si>
+    <t>Sitazid 50mg Tablet 20's</t>
+  </si>
+  <si>
+    <t>Sitazid 100mg Tablet 10's</t>
+  </si>
+  <si>
+    <t>24's</t>
   </si>
   <si>
     <t>30's</t>
   </si>
   <si>
+    <t>20'S</t>
+  </si>
+  <si>
+    <t>50 's</t>
+  </si>
+  <si>
     <t>20's</t>
   </si>
   <si>
-    <t>42's</t>
-  </si>
-  <si>
-    <t>100's</t>
-  </si>
-  <si>
-    <t>24 's</t>
-  </si>
-  <si>
-    <t>48 's</t>
-  </si>
-  <si>
-    <t>60 's</t>
-  </si>
-  <si>
-    <t>48's</t>
-  </si>
-  <si>
-    <t>100 's</t>
-  </si>
-  <si>
-    <t>500's</t>
-  </si>
-  <si>
-    <t>15gm</t>
+    <t>10's</t>
+  </si>
+  <si>
+    <t>20 's</t>
+  </si>
+  <si>
+    <t>10 's</t>
+  </si>
+  <si>
+    <t>40 's</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,7 +528,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -537,143 +537,143 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>36</v>
@@ -681,206 +681,189 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
-        <v>165</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>